<commit_message>
them mot so chuc nang
</commit_message>
<xml_diff>
--- a/api-info.xlsx
+++ b/api-info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\01. Project\InternetBanking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0F0FE5-387F-45B4-8197-1104557D4570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50D0277-2065-4D15-ABAE-09517B88E7A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>link API</t>
   </si>
@@ -193,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -207,6 +207,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -222,6 +225,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,11 +494,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -602,12 +609,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="4" customFormat="1">
+    <row r="14" spans="1:2" s="4" customFormat="1" ht="45">
       <c r="A14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="99">
+      <c r="B17" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
man hinh tao ng nhan
</commit_message>
<xml_diff>
--- a/api-info.xlsx
+++ b/api-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\01. Project\InternetBanking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CC52AD-3E15-4DE8-9B2A-C2198DA31804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F31CA6-E69D-4A2A-B033-0F0CDB28E614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,8 +523,8 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -611,11 +611,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="4" customFormat="1">
+    <row r="11" spans="1:3" s="4" customFormat="1" ht="120">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
payment và thông báo
</commit_message>
<xml_diff>
--- a/api-info.xlsx
+++ b/api-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\01. Project\InternetBanking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4884026C-72B9-4A42-A532-35CF78B17CE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2654AF02-DC86-47A4-8057-82B4B2A09428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>link API</t>
   </si>
@@ -189,6 +190,20 @@
   <si>
     <t>{
     "idNhacNo":"1",
+}</t>
+  </si>
+  <si>
+    <t>localhost:3000/debt/update-debt</t>
+  </si>
+  <si>
+    <t>{
+    "id":4,
+    "taiKhoanDoi":"admin",
+    "taiKhoanNo":"hiep",
+    "soTien":9000000,
+    "noiDung":"Tien dien",
+    "trangThai":0,
+    "phanHoi":"Khong thich tra"
 }</t>
   </si>
 </sst>
@@ -571,8 +586,8 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,11 +784,11 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="6"/>
@@ -784,11 +799,11 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="6"/>
@@ -799,11 +814,11 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="6"/>
@@ -814,11 +829,11 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="6"/>
@@ -919,16 +934,20 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+    <row r="24" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
nho them api tru tien
</commit_message>
<xml_diff>
--- a/api-info.xlsx
+++ b/api-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\01. Project\InternetBanking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93D3D09-9EB4-4B59-9146-0F415895BE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEA304B-6E17-41D0-A7DA-DA37B93F72AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -596,7 +596,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>